<commit_message>
Fix[back]: Fix excel format compatibility issue
</commit_message>
<xml_diff>
--- a/backend/timesheet-template.xlsx
+++ b/backend/timesheet-template.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="remote_work" sheetId="1" r:id="rId1"/>
     <sheet name="محاسبات" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ماه:</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>واحد/ پروژه:</t>
-  </si>
-  <si>
-    <t>پایدار</t>
   </si>
   <si>
     <t>نام مـدیر:</t>
@@ -654,49 +651,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$B$44" fmlaRange="$B$45:$B$56" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$B$44" fmlaRange="$B$45:$B$56" noThreeD="1" sel="5" val="3"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$C$44" fmlaRange="$C$45:$C$48" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$C$44" fmlaRange="$C$45:$C$48" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1543050" cy="847725"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
@@ -813,6 +776,50 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15738862351" y="38101"/>
+          <a:ext cx="857249" cy="857249"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1017,7 +1024,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="P4" sqref="P4:V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1097,9 +1104,7 @@
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="48" t="s">
-        <v>7</v>
-      </c>
+      <c r="E3" s="48"/>
       <c r="F3" s="48"/>
       <c r="G3" s="48"/>
       <c r="H3" s="3"/>
@@ -1111,7 +1116,7 @@
       <c r="N3" s="46"/>
       <c r="O3" s="41"/>
       <c r="P3" s="47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="47"/>
       <c r="R3" s="29"/>
@@ -1125,49 +1130,49 @@
     </row>
     <row r="4" spans="2:27" ht="66.75" thickBot="1">
       <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="38" t="s">
         <v>22</v>
-      </c>
-      <c r="P4" s="38" t="s">
-        <v>23</v>
       </c>
       <c r="Q4" s="31"/>
       <c r="R4" s="31"/>
@@ -1180,7 +1185,7 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
     </row>
-    <row r="5" spans="2:27" ht="24.75" customHeight="1">
+    <row r="5" spans="2:27" ht="24.75" customHeight="1" thickBot="1">
       <c r="B5" s="12">
         <v>1</v>
       </c>
@@ -1230,7 +1235,7 @@
       <c r="U5" s="31"/>
       <c r="V5" s="32"/>
     </row>
-    <row r="6" spans="2:27" ht="24.75" customHeight="1">
+    <row r="6" spans="2:27" ht="24.75" customHeight="1" thickBot="1">
       <c r="B6" s="12">
         <v>2</v>
       </c>
@@ -2080,7 +2085,7 @@
       <c r="U22" s="31"/>
       <c r="V22" s="32"/>
       <c r="AA22" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:27" ht="24.75" customHeight="1" thickBot="1">
@@ -2736,7 +2741,7 @@
     <row r="36" spans="1:22" ht="24.75" customHeight="1" thickBot="1">
       <c r="A36" s="25"/>
       <c r="B36" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
@@ -2793,15 +2798,15 @@
     <row r="43" spans="1:22" ht="12.75" customHeight="1"/>
     <row r="44" spans="1:22" ht="12.75" hidden="1" customHeight="1">
       <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
         <v>2</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="12.75" hidden="1" customHeight="1">
       <c r="B45" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C45">
         <v>1399</v>
@@ -2809,7 +2814,7 @@
     </row>
     <row r="46" spans="1:22" ht="12.75" hidden="1" customHeight="1">
       <c r="B46" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46">
         <v>1400</v>
@@ -2817,7 +2822,7 @@
     </row>
     <row r="47" spans="1:22" ht="12.75" hidden="1" customHeight="1">
       <c r="B47" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47">
         <v>1401</v>
@@ -2825,7 +2830,7 @@
     </row>
     <row r="48" spans="1:22" ht="12.75" hidden="1" customHeight="1">
       <c r="B48" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48">
         <v>1402</v>
@@ -2833,42 +2838,42 @@
     </row>
     <row r="49" spans="2:2" ht="12.75" hidden="1" customHeight="1">
       <c r="B49" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="12.75" hidden="1" customHeight="1">
       <c r="B50" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="12.75" hidden="1" customHeight="1">
       <c r="B51" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="12.75" hidden="1" customHeight="1">
       <c r="B52" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="12.75" hidden="1" customHeight="1">
       <c r="B53" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="12.75" hidden="1" customHeight="1">
       <c r="B54" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="12.75" hidden="1" customHeight="1">
       <c r="B55" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="12.75" hidden="1" customHeight="1">
       <c r="B56" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="12.75" customHeight="1">

</xml_diff>

<commit_message>
removal of drawing shape
</commit_message>
<xml_diff>
--- a/backend/timesheet-template.xlsx
+++ b/backend/timesheet-template.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erfani\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SahaBee\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC39BC5-D881-4CDC-B259-46B2FBF3CD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="remote_work" sheetId="1" r:id="rId1"/>
     <sheet name="محاسبات" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,8 +33,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - Table1" description="Connection to the 'Table1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Table1" description="Connection to the 'Table1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Table1;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table1]"/>
   </connection>
 </connections>
@@ -154,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17">
     <font>
       <sz val="10"/>
@@ -683,7 +688,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0651C89F-09BB-41A3-8C38-0C986D055222}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -741,7 +746,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91116477-02CE-4FF1-A017-13F07397B0E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -776,50 +781,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15738862351" y="38101"/>
-          <a:ext cx="857249" cy="857249"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1020,11 +981,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:V4"/>
+      <selection activeCell="P5" sqref="P5:V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3939,7 +3900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">

</xml_diff>

<commit_message>
Fix[back]: Remove drawing shape in excel template (#26)
Co-authored-by: Alireza Tabarzadi <a.tabarzadi@inside.sahab.ir>
Co-authored-by: Emran BatmanGhelich <emran.bm@gmail.com>
</commit_message>
<xml_diff>
--- a/backend/timesheet-template.xlsx
+++ b/backend/timesheet-template.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erfani\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SahaBee\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC39BC5-D881-4CDC-B259-46B2FBF3CD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="remote_work" sheetId="1" r:id="rId1"/>
     <sheet name="محاسبات" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,8 +33,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - Table1" description="Connection to the 'Table1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Table1" description="Connection to the 'Table1' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Table1;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table1]"/>
   </connection>
 </connections>
@@ -154,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17">
     <font>
       <sz val="10"/>
@@ -683,7 +688,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0651C89F-09BB-41A3-8C38-0C986D055222}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -741,7 +746,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91116477-02CE-4FF1-A017-13F07397B0E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -776,50 +781,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15738862351" y="38101"/>
-          <a:ext cx="857249" cy="857249"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1020,11 +981,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:V4"/>
+      <selection activeCell="P5" sqref="P5:V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3939,7 +3900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">

</xml_diff>